<commit_message>
fixed an issue with # sm molecules counting
</commit_message>
<xml_diff>
--- a/test_short/heatmaps/sm_count.xlsx
+++ b/test_short/heatmaps/sm_count.xlsx
@@ -434,60 +434,38 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>pyridine</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>pyridazine</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>pyrimidine</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>pyrazine</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>pyrrole</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>pyrazole</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>imidazole</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>thiazole</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>oxazole</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>isoxazole</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>furan</t>
-        </is>
+      <c r="A1" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="2">
@@ -495,381 +473,381 @@
         <v>1728</v>
       </c>
       <c r="B2" t="n">
-        <v>121</v>
+        <v>1728</v>
       </c>
       <c r="C2" t="n">
-        <v>434</v>
+        <v>1728</v>
       </c>
       <c r="D2" t="n">
-        <v>144</v>
+        <v>1728</v>
       </c>
       <c r="E2" t="n">
-        <v>543</v>
+        <v>1728</v>
       </c>
       <c r="F2" t="n">
-        <v>1411</v>
+        <v>1728</v>
       </c>
       <c r="G2" t="n">
-        <v>547</v>
+        <v>1728</v>
       </c>
       <c r="H2" t="n">
-        <v>407</v>
+        <v>1728</v>
       </c>
       <c r="I2" t="n">
-        <v>309</v>
+        <v>1728</v>
       </c>
       <c r="J2" t="n">
-        <v>437</v>
+        <v>1728</v>
       </c>
       <c r="K2" t="n">
-        <v>531</v>
+        <v>1728</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1728</v>
+        <v>121</v>
       </c>
       <c r="B3" t="n">
         <v>121</v>
       </c>
       <c r="C3" t="n">
-        <v>434</v>
+        <v>121</v>
       </c>
       <c r="D3" t="n">
-        <v>144</v>
+        <v>121</v>
       </c>
       <c r="E3" t="n">
-        <v>543</v>
+        <v>121</v>
       </c>
       <c r="F3" t="n">
-        <v>1411</v>
+        <v>121</v>
       </c>
       <c r="G3" t="n">
-        <v>547</v>
+        <v>121</v>
       </c>
       <c r="H3" t="n">
-        <v>407</v>
+        <v>121</v>
       </c>
       <c r="I3" t="n">
-        <v>309</v>
+        <v>121</v>
       </c>
       <c r="J3" t="n">
-        <v>437</v>
+        <v>121</v>
       </c>
       <c r="K3" t="n">
-        <v>531</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>1728</v>
+        <v>434</v>
       </c>
       <c r="B4" t="n">
-        <v>121</v>
+        <v>434</v>
       </c>
       <c r="C4" t="n">
         <v>434</v>
       </c>
       <c r="D4" t="n">
-        <v>144</v>
+        <v>434</v>
       </c>
       <c r="E4" t="n">
-        <v>543</v>
+        <v>434</v>
       </c>
       <c r="F4" t="n">
-        <v>1411</v>
+        <v>434</v>
       </c>
       <c r="G4" t="n">
-        <v>547</v>
+        <v>434</v>
       </c>
       <c r="H4" t="n">
-        <v>407</v>
+        <v>434</v>
       </c>
       <c r="I4" t="n">
-        <v>309</v>
+        <v>434</v>
       </c>
       <c r="J4" t="n">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="K4" t="n">
-        <v>531</v>
+        <v>434</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>1728</v>
+        <v>144</v>
       </c>
       <c r="B5" t="n">
-        <v>121</v>
+        <v>144</v>
       </c>
       <c r="C5" t="n">
-        <v>434</v>
+        <v>144</v>
       </c>
       <c r="D5" t="n">
         <v>144</v>
       </c>
       <c r="E5" t="n">
-        <v>543</v>
+        <v>144</v>
       </c>
       <c r="F5" t="n">
-        <v>1411</v>
+        <v>144</v>
       </c>
       <c r="G5" t="n">
-        <v>547</v>
+        <v>144</v>
       </c>
       <c r="H5" t="n">
-        <v>407</v>
+        <v>144</v>
       </c>
       <c r="I5" t="n">
-        <v>309</v>
+        <v>144</v>
       </c>
       <c r="J5" t="n">
-        <v>437</v>
+        <v>144</v>
       </c>
       <c r="K5" t="n">
-        <v>531</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>1728</v>
+        <v>543</v>
       </c>
       <c r="B6" t="n">
-        <v>121</v>
+        <v>543</v>
       </c>
       <c r="C6" t="n">
-        <v>434</v>
+        <v>543</v>
       </c>
       <c r="D6" t="n">
-        <v>144</v>
+        <v>543</v>
       </c>
       <c r="E6" t="n">
         <v>543</v>
       </c>
       <c r="F6" t="n">
-        <v>1411</v>
+        <v>543</v>
       </c>
       <c r="G6" t="n">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="H6" t="n">
-        <v>407</v>
+        <v>543</v>
       </c>
       <c r="I6" t="n">
-        <v>309</v>
+        <v>543</v>
       </c>
       <c r="J6" t="n">
-        <v>437</v>
+        <v>543</v>
       </c>
       <c r="K6" t="n">
-        <v>531</v>
+        <v>543</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>1728</v>
+        <v>1411</v>
       </c>
       <c r="B7" t="n">
-        <v>121</v>
+        <v>1411</v>
       </c>
       <c r="C7" t="n">
-        <v>434</v>
+        <v>1411</v>
       </c>
       <c r="D7" t="n">
-        <v>144</v>
+        <v>1411</v>
       </c>
       <c r="E7" t="n">
-        <v>543</v>
+        <v>1411</v>
       </c>
       <c r="F7" t="n">
         <v>1411</v>
       </c>
       <c r="G7" t="n">
-        <v>547</v>
+        <v>1411</v>
       </c>
       <c r="H7" t="n">
-        <v>407</v>
+        <v>1411</v>
       </c>
       <c r="I7" t="n">
-        <v>309</v>
+        <v>1411</v>
       </c>
       <c r="J7" t="n">
-        <v>437</v>
+        <v>1411</v>
       </c>
       <c r="K7" t="n">
-        <v>531</v>
+        <v>1411</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>1728</v>
+        <v>547</v>
       </c>
       <c r="B8" t="n">
-        <v>121</v>
+        <v>547</v>
       </c>
       <c r="C8" t="n">
-        <v>434</v>
+        <v>547</v>
       </c>
       <c r="D8" t="n">
-        <v>144</v>
+        <v>547</v>
       </c>
       <c r="E8" t="n">
-        <v>543</v>
+        <v>547</v>
       </c>
       <c r="F8" t="n">
-        <v>1411</v>
+        <v>547</v>
       </c>
       <c r="G8" t="n">
         <v>547</v>
       </c>
       <c r="H8" t="n">
-        <v>407</v>
+        <v>547</v>
       </c>
       <c r="I8" t="n">
-        <v>309</v>
+        <v>547</v>
       </c>
       <c r="J8" t="n">
-        <v>437</v>
+        <v>547</v>
       </c>
       <c r="K8" t="n">
-        <v>531</v>
+        <v>547</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>1728</v>
+        <v>407</v>
       </c>
       <c r="B9" t="n">
-        <v>121</v>
+        <v>407</v>
       </c>
       <c r="C9" t="n">
-        <v>434</v>
+        <v>407</v>
       </c>
       <c r="D9" t="n">
-        <v>144</v>
+        <v>407</v>
       </c>
       <c r="E9" t="n">
-        <v>543</v>
+        <v>407</v>
       </c>
       <c r="F9" t="n">
-        <v>1411</v>
+        <v>407</v>
       </c>
       <c r="G9" t="n">
-        <v>547</v>
+        <v>407</v>
       </c>
       <c r="H9" t="n">
         <v>407</v>
       </c>
       <c r="I9" t="n">
-        <v>309</v>
+        <v>407</v>
       </c>
       <c r="J9" t="n">
-        <v>437</v>
+        <v>407</v>
       </c>
       <c r="K9" t="n">
-        <v>531</v>
+        <v>407</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>1728</v>
+        <v>309</v>
       </c>
       <c r="B10" t="n">
-        <v>121</v>
+        <v>309</v>
       </c>
       <c r="C10" t="n">
-        <v>434</v>
+        <v>309</v>
       </c>
       <c r="D10" t="n">
-        <v>144</v>
+        <v>309</v>
       </c>
       <c r="E10" t="n">
-        <v>543</v>
+        <v>309</v>
       </c>
       <c r="F10" t="n">
-        <v>1411</v>
+        <v>309</v>
       </c>
       <c r="G10" t="n">
-        <v>547</v>
+        <v>309</v>
       </c>
       <c r="H10" t="n">
-        <v>407</v>
+        <v>309</v>
       </c>
       <c r="I10" t="n">
         <v>309</v>
       </c>
       <c r="J10" t="n">
-        <v>437</v>
+        <v>309</v>
       </c>
       <c r="K10" t="n">
-        <v>531</v>
+        <v>309</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>1728</v>
+        <v>437</v>
       </c>
       <c r="B11" t="n">
-        <v>121</v>
+        <v>437</v>
       </c>
       <c r="C11" t="n">
-        <v>434</v>
+        <v>437</v>
       </c>
       <c r="D11" t="n">
-        <v>144</v>
+        <v>437</v>
       </c>
       <c r="E11" t="n">
-        <v>543</v>
+        <v>437</v>
       </c>
       <c r="F11" t="n">
-        <v>1411</v>
+        <v>437</v>
       </c>
       <c r="G11" t="n">
-        <v>547</v>
+        <v>437</v>
       </c>
       <c r="H11" t="n">
-        <v>407</v>
+        <v>437</v>
       </c>
       <c r="I11" t="n">
-        <v>309</v>
+        <v>437</v>
       </c>
       <c r="J11" t="n">
         <v>437</v>
       </c>
       <c r="K11" t="n">
-        <v>531</v>
+        <v>437</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>1728</v>
+        <v>531</v>
       </c>
       <c r="B12" t="n">
-        <v>121</v>
+        <v>531</v>
       </c>
       <c r="C12" t="n">
-        <v>434</v>
+        <v>531</v>
       </c>
       <c r="D12" t="n">
-        <v>144</v>
+        <v>531</v>
       </c>
       <c r="E12" t="n">
-        <v>543</v>
+        <v>531</v>
       </c>
       <c r="F12" t="n">
-        <v>1411</v>
+        <v>531</v>
       </c>
       <c r="G12" t="n">
-        <v>547</v>
+        <v>531</v>
       </c>
       <c r="H12" t="n">
-        <v>407</v>
+        <v>531</v>
       </c>
       <c r="I12" t="n">
-        <v>309</v>
+        <v>531</v>
       </c>
       <c r="J12" t="n">
-        <v>437</v>
+        <v>531</v>
       </c>
       <c r="K12" t="n">
         <v>531</v>

</xml_diff>